<commit_message>
feat: in-kind deal structure validated against Al-Malqa (IRR 2.5% delta) + Al-Hada regression pass
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/al_hada_validation.xlsx
+++ b/al_hada_validation.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Assumptions" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="تقرير الأنظمة" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="تقرير أنظمة البناء والتنظيم" sheetId="2" state="visible" r:id="rId2"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="بيانات السوق" sheetId="3" state="visible" r:id="rId3"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="تحليل الحساسية" sheetId="4" state="visible" r:id="rId4"/>
     <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="مقارنة السيناريوهات" sheetId="5" state="visible" r:id="rId5"/>
@@ -649,12 +649,12 @@
     <row r="3">
       <c r="D3" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fund Name </t>
+          <t>Fund Name</t>
         </is>
       </c>
       <c r="E3" s="2" t="inlineStr">
         <is>
-          <t>صندوق استثمار عقاري</t>
+          <t>صندوق استثمار عقاري خاص</t>
         </is>
       </c>
       <c r="L3" s="3" t="inlineStr">
@@ -666,7 +666,7 @@
     <row r="4">
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t xml:space="preserve">Fund Type </t>
+          <t>Fund Type</t>
         </is>
       </c>
       <c r="E4" s="2" t="inlineStr">

</xml_diff>

<commit_message>
fix: brokerage on full price, transfer tax 0 for in-kind deals
Co-authored-by: Cursor <cursoragent@cursor.com>
</commit_message>
<xml_diff>
--- a/al_hada_validation.xlsx
+++ b/al_hada_validation.xlsx
@@ -852,7 +852,7 @@
         <v/>
       </c>
       <c r="H12" s="13">
-        <f>H11*$F$16</f>
+        <f>H11*F12</f>
         <v/>
       </c>
       <c r="I12" s="14">
@@ -912,7 +912,7 @@
         <v>0.05</v>
       </c>
       <c r="F14" s="10">
-        <f>E14*F12</f>
+        <f>IF(I11&gt;0,0,E14*F12)</f>
         <v/>
       </c>
       <c r="L14" s="5" t="inlineStr">
@@ -1297,7 +1297,7 @@
     <row r="35">
       <c r="L35" s="5" t="inlineStr">
         <is>
-          <t>In-Kind Contribution</t>
+          <t>In-Kind (Land Owner)</t>
         </is>
       </c>
       <c r="N35" s="23">
@@ -1313,7 +1313,7 @@
       </c>
       <c r="D36" s="9" t="inlineStr">
         <is>
-          <t>Financing &amp; Fund Cost Assumptions</t>
+          <t>Total Financing &amp; Fund Cost</t>
         </is>
       </c>
       <c r="L36" s="5" t="inlineStr">

</xml_diff>